<commit_message>
CHECK LIST CODIGO APP
Ahi esta
</commit_message>
<xml_diff>
--- a/Prueba 2/CheckList_Inspección de Código.xlsx
+++ b/Prueba 2/CheckList_Inspección de Código.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcela\Desktop\2021\Duoc\Semestre II\PDA221_CSY4111\PDA221_CSY4111\Prueba 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2884d8d705fa78f8/Escritorio/CALIDAD DE SOFTWARE/CHEK LIST DE SUPERMERCADO/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BC5C0FF-06DD-4001-B764-78D0FCF3D572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inspeccion de código" sheetId="2" r:id="rId1"/>
@@ -25,16 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Fecha:</t>
-  </si>
-  <si>
-    <t>Autor:</t>
-  </si>
-  <si>
-    <t>Inspector:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t xml:space="preserve">Ítem </t>
   </si>
@@ -219,13 +211,103 @@
   </si>
   <si>
     <t>CheckList Inspección de Código</t>
+  </si>
+  <si>
+    <t>Fecha: 20/10/2021</t>
+  </si>
+  <si>
+    <t>Autor: Jorge Alfaro Castro</t>
+  </si>
+  <si>
+    <t>Inspector: Matias Fuentealba</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Existe un constructor que es redundante en la case carne</t>
+  </si>
+  <si>
+    <t>Get de atributos de clase Carne</t>
+  </si>
+  <si>
+    <t>Constructor Carne</t>
+  </si>
+  <si>
+    <t>Faltan GET de los atributos de Carne</t>
+  </si>
+  <si>
+    <t>Set de atributos de clase Carne</t>
+  </si>
+  <si>
+    <t>Faltan SET de los atributos de Carne</t>
+  </si>
+  <si>
+    <t>Importacion de packetes de la clase CarritoCompra</t>
+  </si>
+  <si>
+    <t>La importacion de las otras clases a esta esta mal hecha</t>
+  </si>
+  <si>
+    <t>Funcion eliminar producto de CarritoCompra</t>
+  </si>
+  <si>
+    <t>Este metodo no posee la condicion en caso de que el producto a eliminar ya no exista</t>
+  </si>
+  <si>
+    <t>Funcion agregar producto de CarritoCompra</t>
+  </si>
+  <si>
+    <t>Este metodo no posee la condicion en caso de que el producto a agregar ya exista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funcion precio total compra de CarritoCompra </t>
+  </si>
+  <si>
+    <t>La funcion importada "Calcular total pago" esta vacia</t>
+  </si>
+  <si>
+    <t>Constructor Fruta Verdura</t>
+  </si>
+  <si>
+    <t>Existe un constructor que es redundante en la case fruta verdura</t>
+  </si>
+  <si>
+    <t>Get de atributos de Fruta Verdura</t>
+  </si>
+  <si>
+    <t>Faltan GET de los atributos de  fruta verdura</t>
+  </si>
+  <si>
+    <t>Metodos de IMONTOS</t>
+  </si>
+  <si>
+    <t>Los metodos no son usados correctamente en las clases a excepcion de frutas verduras</t>
+  </si>
+  <si>
+    <t>Constructor Producto</t>
+  </si>
+  <si>
+    <t>Existe un constructor que es redundante en la case producto</t>
+  </si>
+  <si>
+    <t>Get y Set de atributos de clase Producto</t>
+  </si>
+  <si>
+    <t>Flata implementar los GET  y SET de la interfaz IMONTOS dentro de la clase Producto</t>
+  </si>
+  <si>
+    <t>Proceso de venta Aplicacion Supermercado</t>
+  </si>
+  <si>
+    <t>Falta calcular total pago frutas y verduras y sumar el precion  de ambos productos con su cantidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,13 +342,62 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -296,13 +427,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -311,15 +438,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="8"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,166 +741,274 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="4.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.6328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="27.453125" customWidth="1"/>
+    <col min="2" max="2" width="4.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.62890625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="82.5234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C1" s="8" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C4" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C5" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="6" t="s">
+      <c r="F7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="7">
+        <v>2</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="7">
+        <v>3</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="7">
+        <v>4</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="7">
+        <v>5</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="7">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="7">
+        <v>7</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="7">
         <v>8</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="6">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="6">
-        <v>3</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="6">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" s="6">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="6">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B14" s="6">
-        <v>7</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="6">
-        <v>8</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B16" s="6">
+      <c r="C15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="7">
         <v>9</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="6">
+      <c r="C16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="7">
         <v>10</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="C17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="7">
+        <v>11</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="7">
+        <v>12</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="7">
+        <v>13</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="13" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="B8:C30">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:C29">
     <sortCondition ref="B8"/>
   </sortState>
   <mergeCells count="1">
@@ -770,38 +1020,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B3" s="5" t="s">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B6" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check list ortogrfia corregida
</commit_message>
<xml_diff>
--- a/Prueba 2/CheckList_Inspección de Código.xlsx
+++ b/Prueba 2/CheckList_Inspección de Código.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2884d8d705fa78f8/Escritorio/CALIDAD DE SOFTWARE/CHEK LIST DE SUPERMERCADO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2884d8d705fa78f8/Escritorio/CALIDAD DE SOFTWARE/MATERIAL PRESENTACION/CALIDAD_DE_SOFTWARE-main/Prueba 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="8_{7BC5C0FF-06DD-4001-B764-78D0FCF3D572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89C66AAD-2740-40B0-AB8A-B1935462E35C}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="8_{7BC5C0FF-06DD-4001-B764-78D0FCF3D572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2307011-3AEA-44B9-90DA-062E7E9AC619}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Observaciones</t>
   </si>
   <si>
-    <t>Nro</t>
-  </si>
-  <si>
     <r>
       <t>·</t>
     </r>
@@ -219,12 +216,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>Este metodo no se pide en modelo de clases</t>
-  </si>
-  <si>
-    <t>setDescuento Categoria()</t>
-  </si>
-  <si>
     <t>toString() en FrutasVerduras y Producto</t>
   </si>
   <si>
@@ -240,9 +231,6 @@
     <t>calcularMontoIva() en FrutaVerdura</t>
   </si>
   <si>
-    <t>Esta clase contiene metodos que no se usan ni se piden</t>
-  </si>
-  <si>
     <t>agregarProducto()</t>
   </si>
   <si>
@@ -261,24 +249,9 @@
     <t>Permite ingresar valor que no son "A", "B" y "C"</t>
   </si>
   <si>
-    <t>Inspector: Matias Fuentealba, Vicente Zurita</t>
-  </si>
-  <si>
     <t>Fecha: 25/10/2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Este metodo utiliza un valor de IVA estatico en vez de los valores de la interfaz y monto </t>
-  </si>
-  <si>
-    <t>El descuento es ingresado de manera manual por el ususario en ves de ser en base  a la categoria del producto</t>
-  </si>
-  <si>
-    <t>Realiza correctamente el calculo, pero no existe un metodo que imprima la informacion</t>
-  </si>
-  <si>
-    <t>Este metodo solo muestra el atributo ''tipo"</t>
-  </si>
-  <si>
     <t>setCategoría()</t>
   </si>
   <si>
@@ -289,6 +262,33 @@
   </si>
   <si>
     <t>Regla de negocio: Cantidad de productos mayor a o igual a 0</t>
+  </si>
+  <si>
+    <t>El descuento es ingresado de manera manual por el usuario en ves de ser en base  a la categoría del producto</t>
+  </si>
+  <si>
+    <t>Inspector: Matías Fuentealba, Vicente Zurita</t>
+  </si>
+  <si>
+    <t>Nro.</t>
+  </si>
+  <si>
+    <t>setDescuento Categoría()</t>
+  </si>
+  <si>
+    <t>Este método no se pide en modelo de clases</t>
+  </si>
+  <si>
+    <t>Realiza correctamente el calculo, pero no existe un método que imprima la información</t>
+  </si>
+  <si>
+    <t>Este método solo muestra el atributo ''tipo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este método utiliza un valor de IVA estático en vez de los valores de la interfaz y monto </t>
+  </si>
+  <si>
+    <t>Esta clase contiene métodos que no se usan ni se piden</t>
   </si>
 </sst>
 </file>
@@ -575,9 +575,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -614,6 +611,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,7 +897,7 @@
   <dimension ref="B1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -908,251 +908,251 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C1" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="C1" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="7" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="22">
+      <c r="B8" s="21">
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="21">
+        <v>2</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="22">
-        <v>2</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="21">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="22">
-        <v>3</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="23" t="s">
-        <v>32</v>
+      <c r="G10" s="22" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="22">
+      <c r="B11" s="21">
         <v>4</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="23" t="s">
-        <v>33</v>
+      <c r="G11" s="22" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="22">
+      <c r="B12" s="21">
         <v>5</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="23" t="s">
-        <v>35</v>
+      <c r="G12" s="22" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="22">
+      <c r="B13" s="21">
         <v>6</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="23" t="s">
-        <v>30</v>
+      <c r="G13" s="22" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="22">
+      <c r="B14" s="21">
         <v>7</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
       <c r="F14" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="22">
+      <c r="B15" s="21">
         <v>8</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="23"/>
+      <c r="G15" s="22"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="22">
+      <c r="B16" s="21">
         <v>9</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D16" s="12"/>
-      <c r="E16" s="16" t="s">
-        <v>13</v>
+      <c r="E16" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="23" t="s">
-        <v>25</v>
+      <c r="G16" s="22" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="22">
+      <c r="B17" s="21">
         <v>10</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17" s="8"/>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="21">
+        <v>11</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="22">
-        <v>11</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>34</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="21">
+        <v>12</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="24"/>
+    </row>
+    <row r="20" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B20" s="25">
         <v>13</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="22">
-        <v>12</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B20" s="26">
-        <v>13</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="31"/>
+      <c r="C20" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" s="11"/>
@@ -1181,27 +1181,27 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>